<commit_message>
Operation Chaining 4ns vivado report aggiornati
</commit_message>
<xml_diff>
--- a/reports/vivado/OperationChaining4nsSolution/power/OperationChaining4nsDSPPowerReport.xlsx
+++ b/reports/vivado/OperationChaining4nsSolution/power/OperationChaining4nsDSPPowerReport.xlsx
@@ -172,7 +172,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
-        <v>2.4706084514036775E-4</v>
+        <v>2.534235536586493E-4</v>
       </c>
       <c r="B2" t="s" s="4">
         <v>8</v>
@@ -198,7 +198,7 @@
     </row>
     <row r="3" outlineLevel="1">
       <c r="A3" t="n" s="5">
-        <v>1.1571797222131863E-4</v>
+        <v>1.1716933659045026E-4</v>
       </c>
       <c r="B3" t="s" s="4">
         <v>10</v>
@@ -219,12 +219,12 @@
         <v>13</v>
       </c>
       <c r="H3" t="n" s="2">
-        <v>5.31076717376709</v>
+        <v>5.329891204833984</v>
       </c>
     </row>
     <row r="4" outlineLevel="1">
       <c r="A4" t="n" s="5">
-        <v>9.711328311823308E-5</v>
+        <v>1.020246054395102E-4</v>
       </c>
       <c r="B4" t="s" s="4">
         <v>14</v>
@@ -245,7 +245,7 @@
         <v>13</v>
       </c>
       <c r="H4" t="n" s="2">
-        <v>4.47619104385376</v>
+        <v>4.539682865142822</v>
       </c>
     </row>
     <row r="5" outlineLevel="1">

</xml_diff>